<commit_message>
Improved findBestN uses low/high range
Values at 6ksps (MorseGenDevice)
5-50 N=44, bw = 136
50-100 N=19, bw = 315
100-200 N=9, bw = 666
</commit_message>
<xml_diff>
--- a/plugins/MorseDigitalModem/morseWpmTcw.xlsx
+++ b/plugins/MorseDigitalModem/morseWpmTcw.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="0" windowWidth="20520" windowHeight="14660" tabRatio="500" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="149">
   <si>
     <t>Mark: 264150</t>
   </si>
@@ -445,9 +445,6 @@
     <t>Res per</t>
   </si>
   <si>
-    <t>Max speed with 4 results per Tcw</t>
-  </si>
-  <si>
     <t>Min results per Tcw</t>
   </si>
   <si>
@@ -455,6 +452,21 @@
   </si>
   <si>
     <t>Var for table</t>
+  </si>
+  <si>
+    <t>Tone</t>
+  </si>
+  <si>
+    <t>Est N gives us N for the minum number of results we want</t>
+  </si>
+  <si>
+    <t>But we also want N to be as large as possible to get narrow bandwidth</t>
+  </si>
+  <si>
+    <t>Try resPerTcw from 12 to 4, looking for bw from 100 to 300</t>
+  </si>
+  <si>
+    <t>Each range doubles the bw</t>
   </si>
 </sst>
 </file>
@@ -510,7 +522,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -534,8 +546,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -548,8 +580,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -561,6 +602,16 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -572,6 +623,16 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1431,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1556,14 +1617,14 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1594,7 +1655,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>131</v>
@@ -1607,18 +1668,19 @@
       </c>
       <c r="G19" s="1">
         <f>$A$19/F19</f>
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="H19" s="1">
         <f>F19*$A$20</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1">
-        <v>0.125</v>
+        <f>1000/A19</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>132</v>
@@ -1631,11 +1693,11 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" ref="G20:G22" si="0">$A$19/F20</f>
-        <v>500</v>
+        <v>375</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" ref="H20:H21" si="1">F20*$A$20</f>
-        <v>2</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1643,7 +1705,7 @@
     <row r="21" spans="1:11">
       <c r="A21" s="1">
         <f>A19/A18</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>133</v>
@@ -1656,21 +1718,21 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="0"/>
-        <v>333.33333333333331</v>
+        <v>250</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1680,18 +1742,22 @@
       </c>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>187.5</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" ref="H22" si="2">F22*$A$20</f>
-        <v>4</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1700,11 +1766,11 @@
       </c>
       <c r="G23" s="1">
         <f>$A$19/F23</f>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="H23" s="1">
         <f>F23*$A$20</f>
-        <v>5</v>
+        <v>6.6666666666666661</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1720,11 +1786,11 @@
       </c>
       <c r="G24" s="1">
         <f>$A$19/F24</f>
-        <v>166.66666666666666</v>
+        <v>125</v>
       </c>
       <c r="H24" s="1">
         <f>F24*$A$20</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1740,11 +1806,11 @@
       </c>
       <c r="G25" s="1">
         <f>$A$19/F25</f>
-        <v>125</v>
+        <v>93.75</v>
       </c>
       <c r="H25" s="1">
         <f>F25*$A$20</f>
-        <v>8</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1760,11 +1826,11 @@
       </c>
       <c r="G26" s="1">
         <f>$A$19/F26</f>
-        <v>111.11111111111111</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="H26" s="1">
         <f>F26*$A$20</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1780,11 +1846,11 @@
       </c>
       <c r="G27" s="1">
         <f>$A$19/F27</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H27" s="1">
         <f>F27*$A$20</f>
-        <v>10</v>
+        <v>13.333333333333332</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1824,6 +1890,9 @@
       <c r="H29" s="5" t="s">
         <v>140</v>
       </c>
+      <c r="J29" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="17" customHeight="1">
       <c r="A30" s="3" t="s">
@@ -1851,7 +1920,9 @@
         <v>124</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="J30" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" ht="17" customHeight="1">
@@ -1880,7 +1951,9 @@
         <v>126</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" ht="17" customHeight="1">
@@ -1893,29 +1966,30 @@
       </c>
       <c r="C32">
         <f>B32/$A$22</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <f>C32/$A$20</f>
-        <v>480</v>
+        <v>180</v>
       </c>
       <c r="E32">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F32">
         <f>E32*$A$20</f>
-        <v>2.5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G32">
         <f>$A$19/E32</f>
-        <v>400</v>
+        <v>136.36363636363637</v>
       </c>
       <c r="H32">
         <f>B32/F32</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="17" customHeight="1">
+        <v>32.727272727272727</v>
+      </c>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" ht="17" customHeight="1">
       <c r="A33">
         <v>10</v>
       </c>
@@ -1924,30 +1998,30 @@
         <v>120</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:C44" si="4">B33/$A$22</f>
-        <v>30</v>
+        <f t="shared" ref="C33:C50" si="4">B33/$A$22</f>
+        <v>15</v>
       </c>
       <c r="D33">
-        <f t="shared" ref="D33:D44" si="5">C33/$A$20</f>
-        <v>240</v>
+        <f t="shared" ref="D33:D50" si="5">C33/$A$20</f>
+        <v>90</v>
       </c>
       <c r="E33">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F33">
-        <f t="shared" ref="F33:F44" si="6">E33*$A$20</f>
-        <v>2.5</v>
+        <f t="shared" ref="F33:F50" si="6">E33*$A$20</f>
+        <v>7.333333333333333</v>
       </c>
       <c r="G33">
-        <f t="shared" ref="G33:G44" si="7">$A$19/E33</f>
-        <v>400</v>
+        <f t="shared" ref="G33:G50" si="7">$A$19/E33</f>
+        <v>136.36363636363637</v>
       </c>
       <c r="H33">
-        <f t="shared" ref="H33:H44" si="8">B33/F33</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <f t="shared" ref="H33:H50" si="8">B33/F33</f>
+        <v>16.363636363636363</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>20</v>
       </c>
@@ -1957,349 +2031,541 @@
       </c>
       <c r="C34">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="D34">
         <f t="shared" si="5"/>
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="E34">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F34">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G34">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>136.36363636363637</v>
       </c>
       <c r="H34">
         <f t="shared" si="8"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>8.1818181818181817</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <f>INT(60/(A35*50)*1000)</f>
+        <v>48</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35" si="9">B35/$A$22</f>
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35" si="10">C35/$A$20</f>
+        <v>36</v>
+      </c>
+      <c r="E35">
+        <v>44</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35" si="11">E35*$A$20</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35" si="12">$A$19/E35</f>
+        <v>136.36363636363637</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35" si="13">B35/F35</f>
+        <v>6.5454545454545459</v>
+      </c>
+      <c r="J35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
         <v>30</v>
       </c>
-      <c r="B35">
-        <f t="shared" ref="B35:B44" si="9">INT(60/(A35*50)*1000)</f>
+      <c r="B36">
+        <f t="shared" ref="B36:B50" si="14">INT(60/(A36*50)*1000)</f>
         <v>40</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="E35">
-        <v>20</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="7"/>
-        <v>400</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36">
-        <v>40</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="9"/>
-        <v>30</v>
       </c>
       <c r="C36">
         <f t="shared" si="4"/>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="D36">
         <f t="shared" si="5"/>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E36">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F36">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G36">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>136.36363636363637</v>
       </c>
       <c r="H36">
         <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>5.454545454545455</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B37">
-        <f t="shared" si="9"/>
-        <v>24</v>
+        <f t="shared" si="14"/>
+        <v>30</v>
       </c>
       <c r="C37">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="D37">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>22.5</v>
       </c>
       <c r="E37">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F37">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G37">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>136.36363636363637</v>
       </c>
       <c r="H37">
         <f t="shared" si="8"/>
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>4.0909090909090908</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B38">
-        <f t="shared" si="9"/>
-        <v>20</v>
+        <f t="shared" ref="B38" si="15">INT(60/(A38*50)*1000)</f>
+        <v>24</v>
       </c>
       <c r="C38">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" ref="C38" si="16">B38/$A$22</f>
+        <v>3</v>
       </c>
       <c r="D38">
-        <f t="shared" si="5"/>
-        <v>40</v>
+        <f t="shared" ref="D38" si="17">C38/$A$20</f>
+        <v>18</v>
       </c>
       <c r="E38">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F38">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
+        <f t="shared" ref="F38" si="18">E38*$A$20</f>
+        <v>7.333333333333333</v>
       </c>
       <c r="G38">
-        <f t="shared" si="7"/>
-        <v>400</v>
+        <f t="shared" ref="G38" si="19">$A$19/E38</f>
+        <v>136.36363636363637</v>
       </c>
       <c r="H38">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39">
-        <v>70</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="9"/>
-        <v>17</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="4"/>
-        <v>4.25</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="5"/>
-        <v>34</v>
-      </c>
-      <c r="E39">
-        <v>20</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="7"/>
-        <v>400</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="8"/>
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <f t="shared" ref="H38" si="20">B38/F38</f>
+        <v>3.2727272727272729</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B40">
-        <f t="shared" si="9"/>
-        <v>15</v>
+        <f t="shared" si="14"/>
+        <v>24</v>
       </c>
       <c r="C40">
         <f t="shared" si="4"/>
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="D40">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E40">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F40">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G40">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>315.78947368421052</v>
       </c>
       <c r="H40">
         <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>7.5789473684210531</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B41">
-        <f t="shared" si="9"/>
-        <v>13</v>
+        <f t="shared" si="14"/>
+        <v>20</v>
       </c>
       <c r="C41">
         <f t="shared" si="4"/>
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="D41">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E41">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F41">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G41">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>315.78947368421052</v>
       </c>
       <c r="H41">
         <f t="shared" si="8"/>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>6.3157894736842106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B42">
-        <f t="shared" si="9"/>
-        <v>12</v>
+        <f t="shared" ref="B42" si="21">INT(60/(A42*50)*1000)</f>
+        <v>17</v>
       </c>
       <c r="C42">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" ref="C42" si="22">B42/$A$22</f>
+        <v>2.125</v>
       </c>
       <c r="D42">
-        <f t="shared" si="5"/>
-        <v>24</v>
+        <f t="shared" ref="D42" si="23">C42/$A$20</f>
+        <v>12.75</v>
       </c>
       <c r="E42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
+        <f t="shared" ref="F42" si="24">E42*$A$20</f>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G42">
-        <f t="shared" si="7"/>
-        <v>400</v>
+        <f t="shared" ref="G42" si="25">$A$19/E42</f>
+        <v>315.78947368421052</v>
       </c>
       <c r="H42">
-        <f t="shared" si="8"/>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <f t="shared" ref="H42" si="26">B42/F42</f>
+        <v>5.3684210526315788</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="B43">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f t="shared" si="14"/>
+        <v>16</v>
       </c>
       <c r="C43">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D43">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E43">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G43">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>315.78947368421052</v>
       </c>
       <c r="H43">
         <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="I43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>5.052631578947369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B44">
-        <f t="shared" si="9"/>
-        <v>9</v>
+        <f t="shared" si="14"/>
+        <v>15</v>
       </c>
       <c r="C44">
         <f t="shared" si="4"/>
-        <v>2.25</v>
+        <v>1.875</v>
       </c>
       <c r="D44">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>11.25</v>
       </c>
       <c r="E44">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F44">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G44">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>315.78947368421052</v>
       </c>
       <c r="H44">
         <f t="shared" si="8"/>
-        <v>3.6</v>
+        <v>4.7368421052631584</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>90</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="4"/>
+        <v>1.625</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="5"/>
+        <v>9.75</v>
+      </c>
+      <c r="E45">
+        <v>19</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="6"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="7"/>
+        <v>315.78947368421052</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="8"/>
+        <v>4.1052631578947372</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46">
+        <v>100</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="E46">
+        <v>19</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="6"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="7"/>
+        <v>315.78947368421052</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="8"/>
+        <v>3.7894736842105265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48">
+        <v>100</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ref="B48" si="27">INT(60/(A48*50)*1000)</f>
+        <v>12</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48" si="28">B48/$A$22</f>
+        <v>1.5</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48" si="29">C48/$A$20</f>
+        <v>9</v>
+      </c>
+      <c r="E48">
+        <v>9</v>
+      </c>
+      <c r="F48">
+        <f t="shared" ref="F48" si="30">E48*$A$20</f>
+        <v>1.5</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ref="G48" si="31">$A$19/E48</f>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48" si="32">B48/F48</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>110</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ref="B49" si="33">INT(60/(A49*50)*1000)</f>
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49" si="34">B49/$A$22</f>
+        <v>1.25</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49" si="35">C49/$A$20</f>
+        <v>7.5</v>
+      </c>
+      <c r="E49">
+        <v>9</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ref="F49" si="36">E49*$A$20</f>
+        <v>1.5</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49" si="37">$A$19/E49</f>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49" si="38">B49/F49</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>120</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>7.5</v>
+      </c>
+      <c r="E50">
+        <v>9</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="7"/>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="8"/>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>150</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ref="B51" si="39">INT(60/(A51*50)*1000)</f>
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51" si="40">B51/$A$22</f>
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51" si="41">C51/$A$20</f>
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <f t="shared" ref="F51" si="42">E51*$A$20</f>
+        <v>1.5</v>
+      </c>
+      <c r="G51">
+        <f t="shared" ref="G51" si="43">$A$19/E51</f>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="H51">
+        <f t="shared" ref="H51" si="44">B51/F51</f>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>200</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ref="B52" si="45">INT(60/(A52*50)*1000)</f>
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52" si="46">B52/$A$22</f>
+        <v>0.75</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ref="D52" si="47">C52/$A$20</f>
+        <v>4.5</v>
+      </c>
+      <c r="E52">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <f t="shared" ref="F52" si="48">E52*$A$20</f>
+        <v>1.5</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ref="G52" si="49">$A$19/E52</f>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="H52">
+        <f t="shared" ref="H52" si="50">B52/F52</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>